<commit_message>
intermediate revision - backport of the changes from junit-dataproviders
</commit_message>
<xml_diff>
--- a/data_2007.xlsx
+++ b/data_2007.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -149,7 +149,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,7 +212,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
intermediate revision - made datafile path attribute more flexible
</commit_message>
<xml_diff>
--- a/data_2007.xlsx
+++ b/data_2007.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">spock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">there is no such thing</t>
   </si>
 </sst>
 </file>
@@ -141,17 +138,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.85714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -198,17 +195,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>